<commit_message>
Noch n Bild in LaTeX
</commit_message>
<xml_diff>
--- a/Abgabe/Model Doku Master.xlsx
+++ b/Abgabe/Model Doku Master.xlsx
@@ -1,28 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Bildverarbeitung_Vorlesung\Abgabe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasbraig/Documents/VSCode/Bildverarbeitung_Vorlesung/Abgabe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{34CE34D1-CCE8-4E57-9FAB-1F9754309545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305068BB-11ED-BC44-B3F4-D7D5CD20633C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{49D3DC9D-7CC7-48E6-A437-E9B65023B1ED}"/>
+    <workbookView xWindow="16740" yWindow="580" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{49D3DC9D-7CC7-48E6-A437-E9B65023B1ED}"/>
   </bookViews>
   <sheets>
     <sheet name="5 Epochen" sheetId="1" r:id="rId1"/>
     <sheet name="30 Epochen" sheetId="3" r:id="rId2"/>
-    <sheet name="60 Epochen" sheetId="2" r:id="rId3"/>
+    <sheet name="30_100px_win" sheetId="4" r:id="rId3"/>
+    <sheet name="60 Epochen" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
   <si>
     <t>epoch</t>
   </si>
@@ -235,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,16 +733,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1424,6 +1437,655 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Loss und Accuracy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'30_100px_win'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>epoch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="76000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'30 Epochen'!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'30_100px_win'!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.65311241149902299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64146190881729104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60405063629150302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51302468776702803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.438176900148391</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39999765157699502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36371305584907498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29016506671905501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.350771814584732</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.31612259149551297</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.73604571819305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.287471503019332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.217108264565467</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.31307935714721602</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.190007269382476</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.176151752471923</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.109340742230415</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4086586236953694E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.118345469236373</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6864355206489501E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.7608541101217201E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.111775524914264</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.1842057406902299E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.45089936256408E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9899733364581999E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.6703585162758799E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6229850482195598E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8229529960080901E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5353727182373399E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7278377092443401E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9735-0D49-B4A5-00B3FC76FE96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'30_100px_win'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>epoch_acc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="77000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'30_100px_win'!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.65805286169052102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65805286169052102</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69471156597137396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76141828298568703</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81670671701431197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84735578298568703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84435093402862504</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8828125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.85516828298568703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.87079328298568703</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48497596383094699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.87079328298568703</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91165864467620805</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.84134614467620805</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.93629807233810403</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.93629807233810403</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95192307233810403</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97836536169052102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95372593402862504</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98858171701431197</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97836536169052102</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95192307233810403</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.97115385532379095</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.98557692766189497</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99459135532379095</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99639421701431197</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9735-0D49-B4A5-00B3FC76FE96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="234555856"/>
+        <c:axId val="234556816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="234555856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="234556816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="234556816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="234555856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -2557,6 +3219,12 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3100,6 +3768,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3644,6 +4815,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB06D385-2CDA-414D-A9D2-5C3E1411F71E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4003,29 +5217,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57BFDCE-30F9-4D46-B74D-2AA05CFB7DFB}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.25" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="4" customWidth="1"/>
     <col min="2" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -4038,8 +5252,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -4052,8 +5266,8 @@
         <v>45711.028113425928</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="6">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -4066,8 +5280,8 @@
         <v>45711.030902777777</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -4080,8 +5294,8 @@
         <v>45711.033726851849</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -4094,8 +5308,8 @@
         <v>45711.036678240744</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -4107,11 +5321,6 @@
       <c r="D7" s="1">
         <v>45711.039444444446</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4125,20 +5334,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8158590-F3A6-4765-A299-96A4AC379C04}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4151,8 +5360,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2">
@@ -4165,8 +5374,8 @@
         <v>45711.061736111114</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3">
@@ -4179,8 +5388,8 @@
         <v>45711.064502314817</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="6">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4">
@@ -4193,8 +5402,8 @@
         <v>45711.067118055558</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5">
@@ -4207,8 +5416,8 @@
         <v>45711.069722222222</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6">
@@ -4221,8 +5430,8 @@
         <v>45711.072326388887</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7">
@@ -4235,8 +5444,8 @@
         <v>45711.074942129628</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="6">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8">
@@ -4249,8 +5458,8 @@
         <v>45711.077546296299</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="6">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9">
@@ -4263,8 +5472,8 @@
         <v>45711.08016203704</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="6">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10">
@@ -4277,8 +5486,8 @@
         <v>45711.082777777781</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="6">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11">
@@ -4291,8 +5500,8 @@
         <v>45711.085393518515</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="6">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12">
@@ -4305,8 +5514,8 @@
         <v>45711.087997685187</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="6">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13">
@@ -4319,8 +5528,8 @@
         <v>45711.090613425928</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="6">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14">
@@ -4333,8 +5542,8 @@
         <v>45711.093229166669</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="6">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15">
@@ -4347,8 +5556,8 @@
         <v>45711.09584490741</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="6">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16">
@@ -4361,8 +5570,8 @@
         <v>45711.098460648151</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="6">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17">
@@ -4375,8 +5584,8 @@
         <v>45711.101076388892</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="6">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18">
@@ -4389,8 +5598,8 @@
         <v>45711.103680555556</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="6">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19">
@@ -4403,8 +5612,8 @@
         <v>45711.106296296297</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="6">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20">
@@ -4417,8 +5626,8 @@
         <v>45711.108912037038</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="6">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21">
@@ -4431,8 +5640,8 @@
         <v>45711.111516203702</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="6">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22">
@@ -4445,8 +5654,8 @@
         <v>45711.11414351852</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="6">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23">
@@ -4459,8 +5668,8 @@
         <v>45711.116759259261</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="6">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24">
@@ -4473,8 +5682,8 @@
         <v>45711.119375000002</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="6">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25">
@@ -4487,8 +5696,8 @@
         <v>45711.121990740743</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="6">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="B26">
@@ -4501,8 +5710,8 @@
         <v>45711.124594907407</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="6">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
       <c r="B27">
@@ -4515,8 +5724,8 @@
         <v>45711.127210648148</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="6">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
       <c r="B28">
@@ -4529,8 +5738,8 @@
         <v>45711.129826388889</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="6">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
       <c r="B29">
@@ -4543,8 +5752,8 @@
         <v>45711.132430555554</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="6">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
       <c r="B30">
@@ -4557,8 +5766,8 @@
         <v>45711.135046296295</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="6">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
       <c r="B31">
@@ -4569,6 +5778,463 @@
       </c>
       <c r="D31" s="1">
         <v>45711.137662037036</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28647B75-35A2-E24B-A571-8888C82690DE}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.65311241149902299</v>
+      </c>
+      <c r="C2">
+        <v>0.65805286169052102</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45713.790729166663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.64146190881729104</v>
+      </c>
+      <c r="C3">
+        <v>0.65805286169052102</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45713.793275462966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.60405063629150302</v>
+      </c>
+      <c r="C4">
+        <v>0.69471156597137396</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45713.79582175926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.51302468776702803</v>
+      </c>
+      <c r="C5">
+        <v>0.76141828298568703</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45713.798379629632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.438176900148391</v>
+      </c>
+      <c r="C6">
+        <v>0.81670671701431197</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45713.800925925927</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.39999765157699502</v>
+      </c>
+      <c r="C7">
+        <v>0.84735578298568703</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45713.803483796299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.36371305584907498</v>
+      </c>
+      <c r="C8">
+        <v>0.84435093402862504</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45713.806030092594</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.29016506671905501</v>
+      </c>
+      <c r="C9">
+        <v>0.8828125</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45713.808576388888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.350771814584732</v>
+      </c>
+      <c r="C10">
+        <v>0.85516828298568703</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45713.81113425926</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.31612259149551297</v>
+      </c>
+      <c r="C11">
+        <v>0.87079328298568703</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45713.813680555555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1.73604571819305</v>
+      </c>
+      <c r="C12">
+        <v>0.48497596383094699</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45713.81622685185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.287471503019332</v>
+      </c>
+      <c r="C13">
+        <v>0.87079328298568703</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45713.818773148145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.217108264565467</v>
+      </c>
+      <c r="C14">
+        <v>0.91165864467620805</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45713.821319444447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.31307935714721602</v>
+      </c>
+      <c r="C15">
+        <v>0.84134614467620805</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45713.823877314811</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.190007269382476</v>
+      </c>
+      <c r="C16">
+        <v>0.93629807233810403</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45713.826423611114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.176151752471923</v>
+      </c>
+      <c r="C17">
+        <v>0.93629807233810403</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45713.828981481478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.109340742230415</v>
+      </c>
+      <c r="C18">
+        <v>0.95192307233810403</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45713.83152777778</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>6.4086586236953694E-2</v>
+      </c>
+      <c r="C19">
+        <v>0.97836536169052102</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45713.834074074075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.118345469236373</v>
+      </c>
+      <c r="C20">
+        <v>0.95372593402862504</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45713.836631944447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>3.6864355206489501E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.98858171701431197</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45713.839178240742</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>5.7608541101217201E-2</v>
+      </c>
+      <c r="C22">
+        <v>0.97836536169052102</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45713.841724537036</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.111775524914264</v>
+      </c>
+      <c r="C23">
+        <v>0.95192307233810403</v>
+      </c>
+      <c r="D23" s="1">
+        <v>45713.844282407408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>8.1842057406902299E-2</v>
+      </c>
+      <c r="C24">
+        <v>0.97115385532379095</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45713.846828703703</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>4.45089936256408E-2</v>
+      </c>
+      <c r="C25">
+        <v>0.98557692766189497</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45713.849386574075</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1.9899733364581999E-2</v>
+      </c>
+      <c r="C26">
+        <v>0.99459135532379095</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45713.851956018516</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1.6703585162758799E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.99639421701431197</v>
+      </c>
+      <c r="D27" s="1">
+        <v>45713.854513888888</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>2.6229850482195598E-3</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45713.857083333336</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1.8229529960080901E-3</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45713.8596412037</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>4.5353727182373399E-4</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45713.862210648149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>2.7278377092443401E-4</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45713.86478009259</v>
       </c>
     </row>
   </sheetData>
@@ -4577,7 +6243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D310A-246D-4083-977F-09A8253E80CF}">
   <dimension ref="A1:D61"/>
   <sheetViews>
@@ -4585,16 +6251,16 @@
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4607,8 +6273,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -4621,8 +6287,8 @@
         <v>45711.140451388892</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -4635,8 +6301,8 @@
         <v>45711.143217592595</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="6">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -4649,8 +6315,8 @@
         <v>45711.145995370367</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -4663,8 +6329,8 @@
         <v>45711.14875</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -4677,8 +6343,8 @@
         <v>45711.151516203703</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -4691,8 +6357,8 @@
         <v>45711.154293981483</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="6">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -4705,8 +6371,8 @@
         <v>45711.157060185185</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="6">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -4719,8 +6385,8 @@
         <v>45711.159826388888</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="6">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -4733,8 +6399,8 @@
         <v>45711.162592592591</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="6">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -4747,8 +6413,8 @@
         <v>45711.165358796294</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="6">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -4761,8 +6427,8 @@
         <v>45711.168136574073</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="6">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -4775,8 +6441,8 @@
         <v>45711.170902777776</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="6">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -4789,8 +6455,8 @@
         <v>45711.173680555556</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="6">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -4803,8 +6469,8 @@
         <v>45711.176435185182</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="6">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -4817,8 +6483,8 @@
         <v>45711.179201388892</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="6">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -4831,8 +6497,8 @@
         <v>45711.181967592594</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="6">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -4845,8 +6511,8 @@
         <v>45711.18472222222</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="6">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -4859,8 +6525,8 @@
         <v>45711.187488425923</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="6">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -4873,8 +6539,8 @@
         <v>45711.190243055556</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="6">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -4887,8 +6553,8 @@
         <v>45711.193009259259</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="6">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -4901,8 +6567,8 @@
         <v>45711.195763888885</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="6">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -4915,8 +6581,8 @@
         <v>45711.198530092595</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="6">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -4929,8 +6595,8 @@
         <v>45711.201296296298</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="6">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -4943,8 +6609,8 @@
         <v>45711.204062500001</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="6">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -4957,8 +6623,8 @@
         <v>45711.206817129627</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="6">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -4971,8 +6637,8 @@
         <v>45711.209583333337</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="6">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -4985,8 +6651,8 @@
         <v>45711.21234953704</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="6">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -4999,11 +6665,11 @@
         <v>45711.215115740742</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="6">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="3">
         <v>372493705071.974</v>
       </c>
       <c r="C30" t="s">
@@ -5013,11 +6679,11 @@
         <v>45711.217870370368</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="6">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="3">
         <v>205543801712.33701</v>
       </c>
       <c r="C31" t="s">
@@ -5027,11 +6693,11 @@
         <v>45711.220636574071</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="6">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="3">
         <v>138596506076.28201</v>
       </c>
       <c r="C32" t="s">
@@ -5041,11 +6707,11 @@
         <v>45711.223402777781</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="6">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="3">
         <v>112507841549.813</v>
       </c>
       <c r="C33" t="s">
@@ -5055,11 +6721,11 @@
         <v>45711.226215277777</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="6">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="3">
         <v>9673713975.6441994</v>
       </c>
       <c r="C34" t="s">
@@ -5069,11 +6735,11 @@
         <v>45711.228981481479</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="6">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="3">
         <v>8427449756.7093897</v>
       </c>
       <c r="C35" t="s">
@@ -5083,11 +6749,11 @@
         <v>45711.231736111113</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="6">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
         <v>34</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="3">
         <v>8005661584.3204699</v>
       </c>
       <c r="C36" t="s">
@@ -5097,11 +6763,11 @@
         <v>45711.234502314815</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="6">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
         <v>35</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="3">
         <v>6800532446.5047998</v>
       </c>
       <c r="C37" t="s">
@@ -5111,11 +6777,11 @@
         <v>45711.237256944441</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="6">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
         <v>36</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="3">
         <v>6156401013.8681602</v>
       </c>
       <c r="C38" t="s">
@@ -5125,11 +6791,11 @@
         <v>45711.240023148152</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="6">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
         <v>37</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="3">
         <v>5667672212.4393501</v>
       </c>
       <c r="C39" t="s">
@@ -5139,11 +6805,11 @@
         <v>45711.242789351854</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="6">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
         <v>38</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="3">
         <v>53965354709.362099</v>
       </c>
       <c r="C40" t="s">
@@ -5153,11 +6819,11 @@
         <v>45711.245555555557</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="6">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
         <v>39</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="3">
         <v>4807017376.1516304</v>
       </c>
       <c r="C41" t="s">
@@ -5167,11 +6833,11 @@
         <v>45711.248310185183</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="3">
         <v>468702683.06520301</v>
       </c>
       <c r="C42" t="s">
@@ -5181,11 +6847,11 @@
         <v>45711.251076388886</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="6">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
         <v>41</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="3">
         <v>4289641310.60638</v>
       </c>
       <c r="C43" t="s">
@@ -5195,11 +6861,11 @@
         <v>45711.253842592596</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="6">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
         <v>42</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="3">
         <v>4053726115.6714501</v>
       </c>
       <c r="C44" t="s">
@@ -5209,11 +6875,11 @@
         <v>45711.256608796299</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="6">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
         <v>43</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="3">
         <v>3703806214.6166301</v>
       </c>
       <c r="C45" t="s">
@@ -5223,11 +6889,11 @@
         <v>45711.259375000001</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="6">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
         <v>44</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="3">
         <v>3669720626.9309301</v>
       </c>
       <c r="C46" t="s">
@@ -5237,11 +6903,11 @@
         <v>45711.262141203704</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="6">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
         <v>45</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="3">
         <v>33947001156.775501</v>
       </c>
       <c r="C47" t="s">
@@ -5251,11 +6917,11 @@
         <v>45711.264907407407</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="6">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
         <v>46</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="3">
         <v>3089668325.6287298</v>
       </c>
       <c r="C48" t="s">
@@ -5265,11 +6931,11 @@
         <v>45711.26767361111</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="6">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
         <v>47</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="3">
         <v>2925939725.1735201</v>
       </c>
       <c r="C49" t="s">
@@ -5279,11 +6945,11 @@
         <v>45711.270439814813</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="6">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
         <v>48</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="3">
         <v>29047437237.750198</v>
       </c>
       <c r="C50" t="s">
@@ -5293,11 +6959,11 @@
         <v>45711.273206018515</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="6">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
         <v>49</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="3">
         <v>26584962142.806</v>
       </c>
       <c r="C51" t="s">
@@ -5307,11 +6973,11 @@
         <v>45711.275972222225</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="6">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
         <v>50</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="3">
         <v>25627798549.976398</v>
       </c>
       <c r="C52" t="s">
@@ -5321,11 +6987,11 @@
         <v>45711.278738425928</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="6">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="3">
         <v>2439732952.5527301</v>
       </c>
       <c r="C53" t="s">
@@ -5335,11 +7001,11 @@
         <v>45711.281493055554</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="6">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="3">
         <v>2318159431.5246902</v>
       </c>
       <c r="C54" t="s">
@@ -5349,11 +7015,11 @@
         <v>45711.284259259257</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="6">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
         <v>53</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="3">
         <v>2290712245.6672301</v>
       </c>
       <c r="C55" t="s">
@@ -5363,11 +7029,11 @@
         <v>45711.28702546296</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="6">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
         <v>54</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="3">
         <v>20865927581.326099</v>
       </c>
       <c r="C56" t="s">
@@ -5377,11 +7043,11 @@
         <v>45711.28979166667</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="6">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
         <v>55</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="3">
         <v>20686575226.136398</v>
       </c>
       <c r="C57" t="s">
@@ -5391,11 +7057,11 @@
         <v>45711.292557870373</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="6">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
         <v>56</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="3">
         <v>19956355572.503502</v>
       </c>
       <c r="C58" t="s">
@@ -5405,11 +7071,11 @@
         <v>45711.295324074075</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="6">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
         <v>57</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="3">
         <v>19126291590.509899</v>
       </c>
       <c r="C59" t="s">
@@ -5419,11 +7085,11 @@
         <v>45711.298090277778</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="6">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
         <v>58</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B60" s="3">
         <v>18289648551.2173</v>
       </c>
       <c r="C60" t="s">
@@ -5433,11 +7099,11 @@
         <v>45711.300856481481</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="6">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
         <v>59</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="3">
         <v>16763536905.273199</v>
       </c>
       <c r="C61" t="s">

</xml_diff>